<commit_message>
Need to include alpha beta and gamma values in the manuscript
</commit_message>
<xml_diff>
--- a/LacTissue_Final_Confirmation.xlsx
+++ b/LacTissue_Final_Confirmation.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9B7ACB-C8B8-4076-BC9A-198376AB9223}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9AB58D-F63C-43EB-8815-E9D349E98CA9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{DD09F72E-4848-464E-B080-00BCFE22713D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="kmct4 t test" sheetId="5" r:id="rId2"/>
-    <sheet name="kmct4 anova data" sheetId="4" r:id="rId3"/>
-    <sheet name="kpl t tes" sheetId="3" r:id="rId4"/>
-    <sheet name="kpl anova data" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId2"/>
+    <sheet name="kmct4 t test" sheetId="5" r:id="rId3"/>
+    <sheet name="kmct4 anova data" sheetId="4" r:id="rId4"/>
+    <sheet name="kpl t tes" sheetId="3" r:id="rId5"/>
+    <sheet name="kpl anova data" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="67">
   <si>
     <t>Normal</t>
   </si>
@@ -110,6 +111,132 @@
   </si>
   <si>
     <t>t Critical two-tail</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>kLP</t>
+  </si>
+  <si>
+    <t>kLEfflux</t>
+  </si>
+  <si>
+    <t>RsqrdP</t>
+  </si>
+  <si>
+    <t>RsqrdLac</t>
+  </si>
+  <si>
+    <t>RMSEP</t>
+  </si>
+  <si>
+    <t>RMSELac</t>
+  </si>
+  <si>
+    <t>3.22E-03</t>
+  </si>
+  <si>
+    <t>9.12E-09</t>
+  </si>
+  <si>
+    <t>3.39E-03</t>
+  </si>
+  <si>
+    <t>2.07E-04</t>
+  </si>
+  <si>
+    <t>1.18E-04</t>
+  </si>
+  <si>
+    <t>3.19E-04</t>
+  </si>
+  <si>
+    <t>3.81E-03</t>
+  </si>
+  <si>
+    <t>2.85E-03</t>
+  </si>
+  <si>
+    <t>8.77E-09</t>
+  </si>
+  <si>
+    <t>1.68E-03</t>
+  </si>
+  <si>
+    <t>7.25E-04</t>
+  </si>
+  <si>
+    <t>4.22E-04</t>
+  </si>
+  <si>
+    <t>3.01E-03</t>
+  </si>
+  <si>
+    <t>5.96E-04</t>
+  </si>
+  <si>
+    <t>6.44E-04</t>
+  </si>
+  <si>
+    <t>4.02E-03</t>
+  </si>
+  <si>
+    <t>0.02 ± 1.18E-04</t>
+  </si>
+  <si>
+    <t>0.02 ± 3.19E-04</t>
+  </si>
+  <si>
+    <t>0.02 ± 0.01</t>
+  </si>
+  <si>
+    <t>3.22E-03 ± 2.85E-03</t>
+  </si>
+  <si>
+    <t>14.06 ± 3.13</t>
+  </si>
+  <si>
+    <t>1.52 ± 1.31</t>
+  </si>
+  <si>
+    <t>3.39E-03 ± 3.39E-03</t>
+  </si>
+  <si>
+    <t>0.01 ± 0.01</t>
+  </si>
+  <si>
+    <t>0.03 ± 7.25E-04</t>
+  </si>
+  <si>
+    <t>0.03 ± 4.22E-04</t>
+  </si>
+  <si>
+    <t>0.03 ± 0.02</t>
+  </si>
+  <si>
+    <t>0.996 ± 5.96E-04</t>
+  </si>
+  <si>
+    <t>0.997 ± 6.44E-04</t>
+  </si>
+  <si>
+    <t>0.989 ± 4.02E-03</t>
+  </si>
+  <si>
+    <t>0.956 ± 0.032</t>
+  </si>
+  <si>
+    <t>0.089 ± 0.007</t>
+  </si>
+  <si>
+    <t>0.078 ± 0.009</t>
+  </si>
+  <si>
+    <t>0.146 ± 0.024</t>
+  </si>
+  <si>
+    <t>0.285 ± 0.138</t>
   </si>
 </sst>
 </file>
@@ -218,7 +345,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
@@ -229,6 +356,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -236,7 +364,28 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2372,8 +2521,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="O47" sqref="O47:Q48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3009,7 +3158,7 @@
         <v>1</v>
       </c>
       <c r="B19">
-        <f t="shared" ref="B19:F34" si="0">IF(OR(ABS(B1-M$5)&lt;=0.001*M$5,ABS(B1-M$6)&lt;=0.001*M$6),0,1)</f>
+        <f t="shared" ref="B19:F19" si="0">IF(OR(ABS(B1-M$5)&lt;=0.001*M$5,ABS(B1-M$6)&lt;=0.001*M$6),0,1)</f>
         <v>1</v>
       </c>
       <c r="C19">
@@ -3503,7 +3652,7 @@
         <v>2</v>
       </c>
       <c r="I37" t="e">
-        <f t="shared" ref="I37:I52" si="7">(E19-$Q$10)/($P$10-$Q$10)</f>
+        <f t="shared" ref="I37" si="7">(E19-$Q$10)/($P$10-$Q$10)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="J37">
@@ -3983,6 +4132,601 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8BA74B9-0D47-41C5-815E-E9C7909E4600}">
+  <sheetPr codeName="Sheet6"/>
+  <dimension ref="A1:K31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21:J27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>2.0640388655312435E-2</v>
+      </c>
+      <c r="C2">
+        <v>6.6060702069415042E-3</v>
+      </c>
+      <c r="D2">
+        <v>10.19817103785174</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2">
+        <v>2.9970284817272021E-2</v>
+      </c>
+      <c r="G2">
+        <v>5.9675758819035002E-2</v>
+      </c>
+      <c r="H2">
+        <v>0.99125727760138016</v>
+      </c>
+      <c r="I2">
+        <v>0.97956179148700517</v>
+      </c>
+      <c r="J2">
+        <v>0.12468545960487196</v>
+      </c>
+      <c r="K2">
+        <v>0.19547964693515865</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2.0880814028200623E-2</v>
+      </c>
+      <c r="C3">
+        <v>1.6676558355789704E-2</v>
+      </c>
+      <c r="D3">
+        <v>14.063348195170397</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3">
+        <v>2.7812768190002262E-2</v>
+      </c>
+      <c r="G3">
+        <v>3.3265308637097507E-2</v>
+      </c>
+      <c r="H3">
+        <v>0.99593860477582208</v>
+      </c>
+      <c r="I3">
+        <v>0.98889446950478532</v>
+      </c>
+      <c r="J3">
+        <v>8.8936434717963489E-2</v>
+      </c>
+      <c r="K3">
+        <v>0.14598597123278839</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>2.0141185909877801E-2</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4">
+        <v>1.5218039662941347</v>
+      </c>
+      <c r="E4">
+        <v>9.9105118116061004E-3</v>
+      </c>
+      <c r="F4">
+        <v>2.6737475899886731E-2</v>
+      </c>
+      <c r="G4">
+        <v>6.3762420474985501E-3</v>
+      </c>
+      <c r="H4">
+        <v>0.99702277168016751</v>
+      </c>
+      <c r="I4">
+        <v>0.95587640865020251</v>
+      </c>
+      <c r="J4">
+        <v>7.7706263621669117E-2</v>
+      </c>
+      <c r="K4">
+        <v>0.28451527348591321</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7">
+        <v>5.7996467137492642</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7">
+        <v>1.7506312950913476E-2</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7">
+        <v>6.7099125555603678E-3</v>
+      </c>
+      <c r="J7">
+        <v>2.4304734850480701E-2</v>
+      </c>
+      <c r="K7">
+        <v>3.9980367203449642E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8">
+        <v>5.1081949958759667E-3</v>
+      </c>
+      <c r="D8">
+        <v>3.1336505466131284</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8">
+        <v>1.7246081208688514E-2</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="J8">
+        <v>6.9233951776703617E-3</v>
+      </c>
+      <c r="K8">
+        <v>2.3688513432857924E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9">
+        <v>1.3061469823137535</v>
+      </c>
+      <c r="E9">
+        <v>8.6895127226370942E-3</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9">
+        <v>6.376242047475212E-3</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9">
+        <v>3.2158865150089026E-2</v>
+      </c>
+      <c r="J9">
+        <v>9.1365500589313132E-3</v>
+      </c>
+      <c r="K9">
+        <v>0.13820744247351507</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" t="s">
+        <v>30</v>
+      </c>
+      <c r="K11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="str">
+        <f>_xlfn.CONCAT(ROUND(B2,2), " ± ", B7)</f>
+        <v>0.02 ± 2.07E-04</v>
+      </c>
+      <c r="C12" t="str">
+        <f>_xlfn.CONCAT(ROUND(C2,2), " ± ", C7)</f>
+        <v>0.01 ± 3.81E-03</v>
+      </c>
+      <c r="D12" t="str">
+        <f>_xlfn.CONCAT(ROUND(D2,2), " ± ", ROUND(D7,2))</f>
+        <v>10.2 ± 5.8</v>
+      </c>
+      <c r="E12" t="str">
+        <f>_xlfn.CONCAT(E2, " ± ", E7)</f>
+        <v>9.12E-09 ± 8.77E-09</v>
+      </c>
+      <c r="F12" t="str">
+        <f>_xlfn.CONCAT(ROUND(F2,2), " ± ", F7)</f>
+        <v>0.03 ± 1.68E-03</v>
+      </c>
+      <c r="G12" t="str">
+        <f>_xlfn.CONCAT(ROUND(G2,2), " ± ", ROUND(G7,2))</f>
+        <v>0.06 ± 0.02</v>
+      </c>
+      <c r="H12" t="str">
+        <f>_xlfn.CONCAT(ROUND(H2,3), " ± ", H7)</f>
+        <v>0.991 ± 3.01E-03</v>
+      </c>
+      <c r="I12" t="str">
+        <f>_xlfn.CONCAT(ROUND(I2,3), " ± ", ROUND(I7,3))</f>
+        <v>0.98 ± 0.007</v>
+      </c>
+      <c r="J12" t="str">
+        <f>_xlfn.CONCAT(ROUND(J2,3), " ± ", ROUND(J7,3))</f>
+        <v>0.125 ± 0.024</v>
+      </c>
+      <c r="K12" t="str">
+        <f>_xlfn.CONCAT(ROUND(K2,3), " ± ", ROUND(K7,3))</f>
+        <v>0.195 ± 0.04</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" ref="B13:B14" si="0">_xlfn.CONCAT(ROUND(B3,2), " ± ", B8)</f>
+        <v>0.02 ± 1.18E-04</v>
+      </c>
+      <c r="C13" t="str">
+        <f>_xlfn.CONCAT(ROUND(C3,2), " ± ", ROUND(C8,2))</f>
+        <v>0.02 ± 0.01</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" ref="D13:D14" si="1">_xlfn.CONCAT(ROUND(D3,2), " ± ", ROUND(D8,2))</f>
+        <v>14.06 ± 3.13</v>
+      </c>
+      <c r="E13" t="str">
+        <f>_xlfn.CONCAT(E3, " ± ", E8)</f>
+        <v>3.39E-03 ± 3.39E-03</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" ref="F13:F14" si="2">_xlfn.CONCAT(ROUND(F3,2), " ± ", F8)</f>
+        <v>0.03 ± 7.25E-04</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" ref="G13:G14" si="3">_xlfn.CONCAT(ROUND(G3,2), " ± ", ROUND(G8,2))</f>
+        <v>0.03 ± 0.02</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" ref="H13:I14" si="4">_xlfn.CONCAT(ROUND(H3,3), " ± ", H8)</f>
+        <v>0.996 ± 5.96E-04</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="4"/>
+        <v>0.989 ± 4.02E-03</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" ref="J13:K14" si="5">_xlfn.CONCAT(ROUND(J3,3), " ± ", ROUND(J8,3))</f>
+        <v>0.089 ± 0.007</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="5"/>
+        <v>0.146 ± 0.024</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>0.02 ± 3.19E-04</v>
+      </c>
+      <c r="C14" t="str">
+        <f>_xlfn.CONCAT(C4, " ± ", C9)</f>
+        <v>3.22E-03 ± 2.85E-03</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>1.52 ± 1.31</v>
+      </c>
+      <c r="E14" t="str">
+        <f>_xlfn.CONCAT(ROUND(E4,2), " ± ", ROUND(E9,2))</f>
+        <v>0.01 ± 0.01</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="2"/>
+        <v>0.03 ± 4.22E-04</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="3"/>
+        <v>0.01 ± 0.01</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="4"/>
+        <v>0.997 ± 6.44E-04</v>
+      </c>
+      <c r="I14" t="str">
+        <f>_xlfn.CONCAT(ROUND(I4,3), " ± ", ROUND(I9,3))</f>
+        <v>0.956 ± 0.032</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="5"/>
+        <v>0.078 ± 0.009</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="5"/>
+        <v>0.285 ± 0.138</v>
+      </c>
+    </row>
+    <row r="21" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>2</v>
+      </c>
+      <c r="J21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" t="s">
+        <v>49</v>
+      </c>
+      <c r="J22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>13</v>
+      </c>
+      <c r="I23" t="s">
+        <v>51</v>
+      </c>
+      <c r="J23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>25</v>
+      </c>
+      <c r="I24" t="s">
+        <v>53</v>
+      </c>
+      <c r="J24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>26</v>
+      </c>
+      <c r="I25" t="s">
+        <v>55</v>
+      </c>
+      <c r="J25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>12</v>
+      </c>
+      <c r="I26" t="s">
+        <v>57</v>
+      </c>
+      <c r="J26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>27</v>
+      </c>
+      <c r="I27" t="s">
+        <v>55</v>
+      </c>
+      <c r="J27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>28</v>
+      </c>
+      <c r="I28" t="s">
+        <v>60</v>
+      </c>
+      <c r="J28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H29" t="s">
+        <v>29</v>
+      </c>
+      <c r="I29" t="s">
+        <v>62</v>
+      </c>
+      <c r="J29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H30" t="s">
+        <v>30</v>
+      </c>
+      <c r="I30" t="s">
+        <v>64</v>
+      </c>
+      <c r="J30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H31" t="s">
+        <v>31</v>
+      </c>
+      <c r="I31" t="s">
+        <v>66</v>
+      </c>
+      <c r="J31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:K4">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+      <formula>0.005</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:K9">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>0.005</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97055BDA-DCFB-43FC-A136-A524520CA669}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:C13"/>
@@ -4112,7 +4856,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88E17877-2AD9-489D-A427-371C750705EF}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:B7"/>
@@ -4175,7 +4919,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0438E80-DC22-4133-A756-8654DAF095E1}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C13"/>
@@ -4305,7 +5049,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B238443-320F-4BFF-8BF4-24794721E863}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B7"/>

</xml_diff>

<commit_message>
Got the tissue slice data finalized
</commit_message>
<xml_diff>
--- a/LacTissue_Final_Confirmation.xlsx
+++ b/LacTissue_Final_Confirmation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9AB58D-F63C-43EB-8815-E9D349E98CA9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDFFD203-A828-4497-BDF5-3E3B8F6BA975}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{DD09F72E-4848-464E-B080-00BCFE22713D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="83">
   <si>
     <t>Normal</t>
   </si>
@@ -237,13 +237,61 @@
   </si>
   <si>
     <t>0.285 ± 0.138</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>ϴ</t>
+  </si>
+  <si>
+    <t>Gamma</t>
+  </si>
+  <si>
+    <t>Theta</t>
+  </si>
+  <si>
+    <t>5.27E+08</t>
+  </si>
+  <si>
+    <t>6.18E+08</t>
+  </si>
+  <si>
+    <t>3.71E+08</t>
+  </si>
+  <si>
+    <t>5.91E+07</t>
+  </si>
+  <si>
+    <t>1.30E+08</t>
+  </si>
+  <si>
+    <t>1.91E+08</t>
+  </si>
+  <si>
+    <t>3.33 ± 0.21</t>
+  </si>
+  <si>
+    <t>3.79 ± 0.67</t>
+  </si>
+  <si>
+    <t>19.66 ± 0.61</t>
+  </si>
+  <si>
+    <t>18.46 ± 1.82</t>
+  </si>
+  <si>
+    <t>6.18E+08 ± 1.30E+08</t>
+  </si>
+  <si>
+    <t>3.71E+08 ± 1.91E+08</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,6 +327,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -345,7 +399,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
@@ -357,6 +411,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -2519,10 +2574,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32AA2958-7DD3-436E-BE35-5CF249EB95A9}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q66"/>
+  <dimension ref="A1:T75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2534,7 +2589,7 @@
     <col min="7" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="2">
         <v>2.0996176350587016E-2</v>
       </c>
@@ -2565,8 +2620,17 @@
       <c r="J1">
         <v>9.8545232846897535E-2</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K1">
+        <v>3.891405037620487</v>
+      </c>
+      <c r="L1">
+        <v>18.245612640749187</v>
+      </c>
+      <c r="M1">
+        <v>1159472564.9070084</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>2.0230353285219438E-2</v>
       </c>
@@ -2597,8 +2661,17 @@
       <c r="J2">
         <v>0.17869607104149435</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <v>3.3354897160400583</v>
+      </c>
+      <c r="L2">
+        <v>20.367225632802807</v>
+      </c>
+      <c r="M2">
+        <v>487716610.19846922</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2.1133216040270707E-2</v>
       </c>
@@ -2629,8 +2702,17 @@
       <c r="J3">
         <v>0.25588545451856037</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>4.0664946324419882</v>
+      </c>
+      <c r="L3">
+        <v>17.899261632944903</v>
+      </c>
+      <c r="M3">
+        <v>450367148.26035923</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1.9820491693986659E-2</v>
       </c>
@@ -2661,8 +2743,17 @@
       <c r="J4">
         <v>0.14837446835332921</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>2.829889569591987</v>
+      </c>
+      <c r="L4">
+        <v>18.789486969326333</v>
+      </c>
+      <c r="M4">
+        <v>206769871.46757409</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1.9939235331044407E-2</v>
       </c>
@@ -2693,30 +2784,39 @@
       <c r="J5" s="1">
         <v>0.92654693581325986</v>
       </c>
+      <c r="K5">
+        <v>3.557702514362866</v>
+      </c>
       <c r="L5" s="1">
+        <v>19.588620561507234</v>
+      </c>
+      <c r="M5" s="1">
+        <v>1049609826.8268603</v>
+      </c>
+      <c r="O5">
         <f>1/51</f>
         <v>1.9607843137254902E-2</v>
       </c>
-      <c r="M5" s="1">
+      <c r="P5">
         <v>1E-4</v>
       </c>
-      <c r="N5" s="1">
+      <c r="Q5" s="1">
         <f>10^-8</f>
         <v>1E-8</v>
       </c>
-      <c r="O5" s="1">
+      <c r="R5" s="1">
         <f>10^-20</f>
         <v>9.9999999999999995E-21</v>
       </c>
-      <c r="P5" s="1">
+      <c r="S5" s="1">
         <f>1/38</f>
         <v>2.6315789473684209E-2</v>
       </c>
-      <c r="Q5" s="1">
+      <c r="T5" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>2.049470218904903E-2</v>
       </c>
@@ -2747,28 +2847,37 @@
       <c r="J6">
         <v>9.0334485610375909E-2</v>
       </c>
+      <c r="K6">
+        <v>2.9202809034091346</v>
+      </c>
       <c r="L6">
+        <v>21.152546591509569</v>
+      </c>
+      <c r="M6">
+        <v>378462133.26087624</v>
+      </c>
+      <c r="O6">
         <f>1/47</f>
         <v>2.1276595744680851E-2</v>
       </c>
-      <c r="M6">
+      <c r="P6">
         <v>0.08</v>
       </c>
-      <c r="N6">
+      <c r="Q6">
         <v>25</v>
       </c>
-      <c r="O6">
+      <c r="R6">
         <v>0.1</v>
       </c>
-      <c r="P6">
+      <c r="S6">
         <f>1/20</f>
         <v>0.05</v>
       </c>
-      <c r="Q6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>2.1211388959800601E-2</v>
       </c>
@@ -2799,8 +2908,17 @@
       <c r="J7">
         <v>0.27077327391731437</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>3.9269590737035491</v>
+      </c>
+      <c r="L7">
+        <v>19.062597659260327</v>
+      </c>
+      <c r="M7">
+        <v>635120824.29158974</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>2.0418198121840758E-2</v>
       </c>
@@ -2831,8 +2949,17 @@
       <c r="J8">
         <v>0.13610483430251968</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>3.1577611006006272</v>
+      </c>
+      <c r="L8">
+        <v>21.124798549955376</v>
+      </c>
+      <c r="M8">
+        <v>475597887.4506402</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>2.0715318885806265E-2</v>
       </c>
@@ -2863,8 +2990,17 @@
       <c r="J9">
         <v>0.1573666046037831</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <v>2.9473957348877371</v>
+      </c>
+      <c r="L9">
+        <v>18.832425123574478</v>
+      </c>
+      <c r="M9">
+        <v>239899343.63687354</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>2.0625110187180679E-2</v>
       </c>
@@ -2895,8 +3031,17 @@
       <c r="J10">
         <v>0.24211475717145006</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <v>4.4726563004025124</v>
+      </c>
+      <c r="L10">
+        <v>17.520786148262779</v>
+      </c>
+      <c r="M10">
+        <v>608406169.72654819</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>2.0828777121022858E-2</v>
       </c>
@@ -2927,8 +3072,17 @@
       <c r="J11">
         <v>0.12480884051876322</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <v>2.9656785774720609</v>
+      </c>
+      <c r="L11">
+        <v>21.213169561097558</v>
+      </c>
+      <c r="M11">
+        <v>617081041.21075487</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>2.1193197649676143E-2</v>
       </c>
@@ -2959,8 +3113,17 @@
       <c r="J12">
         <v>0.10320486060620654</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <v>2.9501216064507223</v>
+      </c>
+      <c r="L12">
+        <v>20.641134469222237</v>
+      </c>
+      <c r="M12">
+        <v>764449816.87107611</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>1.9972000811914196E-2</v>
       </c>
@@ -2991,8 +3154,17 @@
       <c r="J13">
         <v>7.062384869236453E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K13">
+        <v>5.074071589865313</v>
+      </c>
+      <c r="L13">
+        <v>15.178948460306106</v>
+      </c>
+      <c r="M13">
+        <v>715521749.05258536</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1.9678783667769612E-2</v>
       </c>
@@ -3023,8 +3195,17 @@
       <c r="J14" s="1">
         <v>1.3349999535357298</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K14">
+        <v>3.8015960996958804</v>
+      </c>
+      <c r="L14">
+        <v>11.970888778378551</v>
+      </c>
+      <c r="M14">
+        <v>9294007.5094139203</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>1.9693401361322888E-2</v>
       </c>
@@ -3055,8 +3236,17 @@
       <c r="J15">
         <v>0.54309124429125588</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K15">
+        <v>2.795149855726895</v>
+      </c>
+      <c r="L15">
+        <v>21.470565518653629</v>
+      </c>
+      <c r="M15">
+        <v>57752389.057093427</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>2.0758155556396315E-2</v>
       </c>
@@ -3086,6 +3276,15 @@
       </c>
       <c r="J16">
         <v>0.23983072747411929</v>
+      </c>
+      <c r="K16">
+        <v>3.5026120946644226</v>
+      </c>
+      <c r="L16">
+        <v>18.719650766396342</v>
+      </c>
+      <c r="M16">
+        <v>338835626.27842277</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -3119,6 +3318,15 @@
       <c r="J17">
         <v>0.32136824912298095</v>
       </c>
+      <c r="K17">
+        <v>4.1712680458839158</v>
+      </c>
+      <c r="L17">
+        <v>19.701405556844808</v>
+      </c>
+      <c r="M17">
+        <v>435197705.82041383</v>
+      </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
@@ -3151,14 +3359,23 @@
       <c r="J18">
         <v>5.8470631985780182E-2</v>
       </c>
+      <c r="K18">
+        <v>3.324544244530617</v>
+      </c>
+      <c r="L18">
+        <v>20.171256983151267</v>
+      </c>
+      <c r="M18">
+        <v>1399632713.5209503</v>
+      </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f>IF(OR(ABS(A1-L$5)&lt;=0.001*L$5,ABS(A1-L$6)&lt;=0.001*L$6),0,1)</f>
+        <f>IF(OR(ABS(A1-O$5)&lt;=0.001*O$5,ABS(A1-O$6)&lt;=0.001*O$6),0,1)</f>
         <v>1</v>
       </c>
       <c r="B19">
-        <f t="shared" ref="B19:F19" si="0">IF(OR(ABS(B1-M$5)&lt;=0.001*M$5,ABS(B1-M$6)&lt;=0.001*M$6),0,1)</f>
+        <f t="shared" ref="B19:F34" si="0">IF(OR(ABS(B1-P$5)&lt;=0.001*P$5,ABS(B1-P$6)&lt;=0.001*P$6),0,1)</f>
         <v>1</v>
       </c>
       <c r="C19">
@@ -3180,27 +3397,27 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f t="shared" ref="A20:A36" si="1">IF(OR(ABS(A2-L$5)&lt;=0.001*L$5,ABS(A2-L$6)&lt;=0.001*L$6),0,1)</f>
+        <f t="shared" ref="A20:A36" si="1">IF(OR(ABS(A2-O$5)&lt;=0.001*O$5,ABS(A2-O$6)&lt;=0.001*O$6),0,1)</f>
         <v>1</v>
       </c>
       <c r="B20">
-        <f t="shared" ref="B20:B36" si="2">IF(OR(ABS(B2-M$5)&lt;=0.001*M$5,ABS(B2-M$6)&lt;=0.001*M$6),0,1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C20">
-        <f t="shared" ref="C20:C36" si="3">IF(OR(ABS(C2-N$5)&lt;=0.001*N$5,ABS(C2-N$6)&lt;=0.001*N$6),0,1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D20">
-        <f t="shared" ref="D20:D36" si="4">IF(OR(ABS(D2-O$5)&lt;=0.001*O$5,ABS(D2-O$6)&lt;=0.001*O$6),0,1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E20">
-        <f t="shared" ref="E20:E36" si="5">IF(OR(ABS(E2-P$5)&lt;=0.001*P$5,ABS(E2-P$6)&lt;=0.001*P$6),0,1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F20">
-        <f t="shared" ref="F20:F36" si="6">IF(OR(ABS(F2-Q$5)&lt;=0.001*Q$5,ABS(F2-Q$6)&lt;=0.001*Q$6),0,1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3210,23 +3427,23 @@
         <v>1</v>
       </c>
       <c r="B21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3236,23 +3453,23 @@
         <v>1</v>
       </c>
       <c r="B22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3262,23 +3479,23 @@
         <v>1</v>
       </c>
       <c r="B23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3288,23 +3505,23 @@
         <v>1</v>
       </c>
       <c r="B24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3314,23 +3531,23 @@
         <v>1</v>
       </c>
       <c r="B25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M25" t="s">
@@ -3346,23 +3563,23 @@
         <v>1</v>
       </c>
       <c r="B26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L26" t="s">
@@ -3381,23 +3598,23 @@
         <v>1</v>
       </c>
       <c r="B27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M27">
@@ -3413,23 +3630,23 @@
         <v>1</v>
       </c>
       <c r="B28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3439,23 +3656,23 @@
         <v>1</v>
       </c>
       <c r="B29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3465,23 +3682,23 @@
         <v>1</v>
       </c>
       <c r="B30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3491,23 +3708,23 @@
         <v>1</v>
       </c>
       <c r="B31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3517,23 +3734,23 @@
         <v>1</v>
       </c>
       <c r="B32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F32">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3543,23 +3760,23 @@
         <v>1</v>
       </c>
       <c r="B33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F33">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3569,23 +3786,23 @@
         <v>1</v>
       </c>
       <c r="B34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3595,23 +3812,23 @@
         <v>1</v>
       </c>
       <c r="B35">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="B35:B36" si="2">IF(OR(ABS(B17-P$5)&lt;=0.001*P$5,ABS(B17-P$6)&lt;=0.001*P$6),0,1)</f>
         <v>1</v>
       </c>
       <c r="C35">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="C35:C36" si="3">IF(OR(ABS(C17-Q$5)&lt;=0.001*Q$5,ABS(C17-Q$6)&lt;=0.001*Q$6),0,1)</f>
         <v>1</v>
       </c>
       <c r="D35">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="D35:D36" si="4">IF(OR(ABS(D17-R$5)&lt;=0.001*R$5,ABS(D17-R$6)&lt;=0.001*R$6),0,1)</f>
         <v>1</v>
       </c>
       <c r="E35">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="E35:E36" si="5">IF(OR(ABS(E17-S$5)&lt;=0.001*S$5,ABS(E17-S$6)&lt;=0.001*S$6),0,1)</f>
         <v>1</v>
       </c>
       <c r="F35">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="F35:F36" si="6">IF(OR(ABS(F17-T$5)&lt;=0.001*T$5,ABS(F17-T$6)&lt;=0.001*T$6),0,1)</f>
         <v>1</v>
       </c>
     </row>
@@ -4058,7 +4275,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="10:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="10:16" x14ac:dyDescent="0.25">
       <c r="J65" t="s">
         <v>10</v>
       </c>
@@ -4075,7 +4292,7 @@
         <v>0.28451527348591321</v>
       </c>
     </row>
-    <row r="66" spans="10:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="10:16" x14ac:dyDescent="0.25">
       <c r="K66">
         <f>STDEV(J$2,J$6,J$7,J$10)/SQRT(COUNT(J$2,J$6,J$7,J$10))</f>
         <v>3.9980367203449642E-2</v>
@@ -4087,6 +4304,132 @@
       <c r="M66">
         <f>STDEV(J$13,J$15,J$16)/SQRT(COUNT(J$13,J$15,J$16))</f>
         <v>0.13820744247351507</v>
+      </c>
+    </row>
+    <row r="67" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="L67" t="s">
+        <v>0</v>
+      </c>
+      <c r="M67" t="s">
+        <v>1</v>
+      </c>
+      <c r="N67" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="K68" t="s">
+        <v>67</v>
+      </c>
+      <c r="L68">
+        <f>AVERAGE(K$2,K$6,K$7,K$10)</f>
+        <v>3.6638464983888133</v>
+      </c>
+      <c r="M68">
+        <f>AVERAGE(K$1,K$8,K$9,K$11,K$12,K$3)</f>
+        <v>3.3298094482456033</v>
+      </c>
+      <c r="N68">
+        <f>AVERAGE(K$13,K$15,K$16)</f>
+        <v>3.7906111800855435</v>
+      </c>
+    </row>
+    <row r="69" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="L69">
+        <f>STDEV(K$2,K$6,K$7,K$10)/SQRT(COUNT(K$2,K$6,K$7,K$10))</f>
+        <v>0.33962105029896961</v>
+      </c>
+      <c r="M69">
+        <f>STDEV(K$1,K$8,K$9,K$11,K$12,K$3)/SQRT(COUNT(K$1,K$8,K$9,K$11,K$12,K$3))</f>
+        <v>0.20902070846118584</v>
+      </c>
+      <c r="N69">
+        <f>STDEV(K$13,K$15,K$16)/SQRT(COUNT(K$13,K$15,K$16))</f>
+        <v>0.67344355677484558</v>
+      </c>
+    </row>
+    <row r="70" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="M70" t="s">
+        <v>0</v>
+      </c>
+      <c r="N70" t="s">
+        <v>1</v>
+      </c>
+      <c r="O70" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="L71" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="M71">
+        <f>AVERAGE(L$2,L$6,L$7,L$10)</f>
+        <v>19.525789007958871</v>
+      </c>
+      <c r="N71">
+        <f>AVERAGE(L$1,L$8,L$9,L$11,L$12,L$3)</f>
+        <v>19.659400329590621</v>
+      </c>
+      <c r="O71">
+        <f>AVERAGE(L$13,L$15,L$16)</f>
+        <v>18.456388248452026</v>
+      </c>
+    </row>
+    <row r="72" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="M72">
+        <f>STDEV(L$2,L$6,L$7,L$10)/SQRT(COUNT(L$2,L$6,L$7,L$10))</f>
+        <v>0.79524307196852007</v>
+      </c>
+      <c r="N72">
+        <f>STDEV(L$1,L$8,L$9,L$11,L$12,L$3)/SQRT(COUNT(L$1,L$8,L$9,L$11,L$12,L$3))</f>
+        <v>0.61389913780302197</v>
+      </c>
+      <c r="O72">
+        <f>STDEV(L$13,L$15,L$16)/SQRT(COUNT(L$13,L$15,L$16))</f>
+        <v>1.8209971322728842</v>
+      </c>
+    </row>
+    <row r="73" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="N73" t="s">
+        <v>0</v>
+      </c>
+      <c r="O73" t="s">
+        <v>1</v>
+      </c>
+      <c r="P73" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="M74" t="s">
+        <v>69</v>
+      </c>
+      <c r="N74">
+        <f>AVERAGE(M$2,M$6,M$7,M$10)</f>
+        <v>527426434.36937082</v>
+      </c>
+      <c r="O74">
+        <f>AVERAGE(M$1,M$8,M$9,M$11,M$12,M$3)</f>
+        <v>617811300.3894521</v>
+      </c>
+      <c r="P74">
+        <f>AVERAGE(M$13,M$15,M$16)</f>
+        <v>370703254.79603386</v>
+      </c>
+    </row>
+    <row r="75" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="N75">
+        <f>STDEV(M$2,M$6,M$7,M$10)/SQRT(COUNT(M$2,M$6,M$7,M$10))</f>
+        <v>59106564.990464196</v>
+      </c>
+      <c r="O75">
+        <f>STDEV(M$1,M$8,M$9,M$11,M$12,M$3)/SQRT(COUNT(M$1,M$8,M$9,M$11,M$12,M$3))</f>
+        <v>129869159.69950381</v>
+      </c>
+      <c r="P75">
+        <f>STDEV(M$13,M$15,M$16)/SQRT(COUNT(M$13,M$15,M$16))</f>
+        <v>190549024.35482064</v>
       </c>
     </row>
   </sheetData>
@@ -4127,32 +4470,34 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8BA74B9-0D47-41C5-815E-E9C7909E4600}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21:J27"/>
+      <selection activeCell="H32" sqref="H32:J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.85546875" customWidth="1"/>
+    <col min="10" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>11</v>
       </c>
@@ -4183,8 +4528,17 @@
       <c r="K1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" t="s">
+        <v>70</v>
+      </c>
+      <c r="N1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4218,8 +4572,17 @@
       <c r="K2">
         <v>0.19547964693515865</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <v>3.6638464983888133</v>
+      </c>
+      <c r="M2">
+        <v>19.525789007958871</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -4253,8 +4616,17 @@
       <c r="K3">
         <v>0.14598597123278839</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <v>3.3298094482456033</v>
+      </c>
+      <c r="M3">
+        <v>19.659400329590621</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -4288,8 +4660,17 @@
       <c r="K4">
         <v>0.28451527348591321</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>3.7906111800855435</v>
+      </c>
+      <c r="M4">
+        <v>18.456388248452026</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -4320,8 +4701,17 @@
       <c r="K6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M6" t="s">
+        <v>70</v>
+      </c>
+      <c r="N6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -4355,8 +4745,17 @@
       <c r="K7">
         <v>3.9980367203449642E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>0.33962105029896961</v>
+      </c>
+      <c r="M7">
+        <v>0.79524307196852007</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -4390,8 +4789,17 @@
       <c r="K8">
         <v>2.3688513432857924E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <v>0.20902070846118584</v>
+      </c>
+      <c r="M8">
+        <v>0.61389913780302197</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -4425,8 +4833,17 @@
       <c r="K9">
         <v>0.13820744247351507</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <v>0.67344355677484558</v>
+      </c>
+      <c r="M9">
+        <v>1.8209971322728842</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>11</v>
       </c>
@@ -4457,8 +4874,17 @@
       <c r="K11" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" t="s">
+        <v>67</v>
+      </c>
+      <c r="M11" t="s">
+        <v>70</v>
+      </c>
+      <c r="N11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -4502,8 +4928,20 @@
         <f>_xlfn.CONCAT(ROUND(K2,3), " ± ", ROUND(K7,3))</f>
         <v>0.195 ± 0.04</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" t="str">
+        <f>_xlfn.CONCAT(ROUND(L2,2), " ± ", ROUND(L7,2))</f>
+        <v>3.66 ± 0.34</v>
+      </c>
+      <c r="M12" t="str">
+        <f>_xlfn.CONCAT(ROUND(M2,2), " ± ", ROUND(M7,2))</f>
+        <v>19.53 ± 0.8</v>
+      </c>
+      <c r="N12" t="str">
+        <f>_xlfn.CONCAT(N2, " ± ", N7)</f>
+        <v>5.27E+08 ± 5.91E+07</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -4547,8 +4985,20 @@
         <f t="shared" si="5"/>
         <v>0.146 ± 0.024</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" t="str">
+        <f t="shared" ref="L13:M14" si="6">_xlfn.CONCAT(ROUND(L3,2), " ± ", ROUND(L8,2))</f>
+        <v>3.33 ± 0.21</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="6"/>
+        <v>19.66 ± 0.61</v>
+      </c>
+      <c r="N13" t="str">
+        <f t="shared" ref="N13:N14" si="7">_xlfn.CONCAT(N3, " ± ", N8)</f>
+        <v>6.18E+08 ± 1.30E+08</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -4592,6 +5042,18 @@
         <f t="shared" si="5"/>
         <v>0.285 ± 0.138</v>
       </c>
+      <c r="L14" t="str">
+        <f t="shared" si="6"/>
+        <v>3.79 ± 0.67</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="6"/>
+        <v>18.46 ± 1.82</v>
+      </c>
+      <c r="N14" t="str">
+        <f t="shared" si="7"/>
+        <v>3.71E+08 ± 1.91E+08</v>
+      </c>
     </row>
     <row r="21" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I21" t="s">
@@ -4709,6 +5171,39 @@
       </c>
       <c r="J31" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H32" t="s">
+        <v>67</v>
+      </c>
+      <c r="I32" t="s">
+        <v>78</v>
+      </c>
+      <c r="J32" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H33" t="s">
+        <v>70</v>
+      </c>
+      <c r="I33" t="s">
+        <v>80</v>
+      </c>
+      <c r="J33" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H34" t="s">
+        <v>69</v>
+      </c>
+      <c r="I34" t="s">
+        <v>82</v>
+      </c>
+      <c r="J34" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added all supplemental figures except for AIC
</commit_message>
<xml_diff>
--- a/LacTissue_Final_Confirmation.xlsx
+++ b/LacTissue_Final_Confirmation.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDFFD203-A828-4497-BDF5-3E3B8F6BA975}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D6BFB5-C5B8-4607-8941-46EC3EA054B1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{DD09F72E-4848-464E-B080-00BCFE22713D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="6" r:id="rId2"/>
-    <sheet name="kmct4 t test" sheetId="5" r:id="rId3"/>
-    <sheet name="kmct4 anova data" sheetId="4" r:id="rId4"/>
-    <sheet name="kpl t tes" sheetId="3" r:id="rId5"/>
-    <sheet name="kpl anova data" sheetId="2" r:id="rId6"/>
+    <sheet name="Sheet3" sheetId="7" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId3"/>
+    <sheet name="kmct4 t test" sheetId="5" r:id="rId4"/>
+    <sheet name="kmct4 anova data" sheetId="4" r:id="rId5"/>
+    <sheet name="kpl t tes" sheetId="3" r:id="rId6"/>
+    <sheet name="kpl anova data" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="86">
   <si>
     <t>Normal</t>
   </si>
@@ -285,13 +286,22 @@
   </si>
   <si>
     <t>3.71E+08 ± 1.91E+08</t>
+  </si>
+  <si>
+    <t>Ok</t>
+  </si>
+  <si>
+    <t>Lower</t>
+  </si>
+  <si>
+    <t>Sample Type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -333,6 +343,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -399,7 +415,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
@@ -412,6 +428,7 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -2577,7 +2594,7 @@
   <dimension ref="A1:T75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+      <selection activeCell="O4" sqref="O4:T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2752,6 +2769,24 @@
       <c r="M4">
         <v>206769871.46757409</v>
       </c>
+      <c r="O4" t="s">
+        <v>11</v>
+      </c>
+      <c r="P4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>25</v>
+      </c>
+      <c r="R4" t="s">
+        <v>26</v>
+      </c>
+      <c r="S4" t="s">
+        <v>12</v>
+      </c>
+      <c r="T4" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -2870,8 +2905,8 @@
         <v>0.1</v>
       </c>
       <c r="S6">
-        <f>1/20</f>
-        <v>0.05</v>
+        <f>1/10</f>
+        <v>0.1</v>
       </c>
       <c r="T6">
         <v>1</v>
@@ -3288,28 +3323,28 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+      <c r="A17" s="10">
         <v>2.0847482463769933E-2</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="10">
         <v>4.0829526313875409E-4</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="10">
         <v>0.4837509499428731</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="10">
         <v>2.340455959641114E-14</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="10">
         <v>2.8052596274836205E-2</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="10">
         <v>2.6477225125270086E-2</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="10">
         <v>0.96215051564743681</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17" s="10">
         <v>0.95334326921431511</v>
       </c>
       <c r="I17">
@@ -3329,28 +3364,28 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+      <c r="A18" s="10">
         <v>2.0247394581427512E-2</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="10">
         <v>7.9999999756638684E-2</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="10">
         <v>4.1171310221576345</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="10">
         <v>3.0119746192602149E-6</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="10">
         <v>4.6370419611511879E-2</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="10">
         <v>0.35853563841044273</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="10">
         <v>0.98905815356158455</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H18" s="10">
         <v>0.99833497706207242</v>
       </c>
       <c r="I18">
@@ -3370,185 +3405,185 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <f>IF(OR(ABS(A1-O$5)&lt;=0.001*O$5,ABS(A1-O$6)&lt;=0.001*O$6),0,1)</f>
-        <v>1</v>
-      </c>
-      <c r="B19">
-        <f t="shared" ref="B19:F34" si="0">IF(OR(ABS(B1-P$5)&lt;=0.001*P$5,ABS(B1-P$6)&lt;=0.001*P$6),0,1)</f>
-        <v>1</v>
-      </c>
-      <c r="C19">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="A19" t="str">
+        <f>_xlfn.IFS(ABS(A1-O$5)&lt;=0.001*O$5,"Lower",ABS(A1-O$6)&lt;=0.001*O$6,"Upper",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" ref="B19:F34" si="0">_xlfn.IFS(ABS(B1-P$5)&lt;=0.001*P$5,"Lower",ABS(B1-P$6)&lt;=0.001*P$6,"Upper",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <f t="shared" ref="A20:A36" si="1">IF(OR(ABS(A2-O$5)&lt;=0.001*O$5,ABS(A2-O$6)&lt;=0.001*O$6),0,1)</f>
-        <v>1</v>
-      </c>
-      <c r="B20">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="A20" t="str">
+        <f t="shared" ref="A20:A36" si="1">_xlfn.IFS(ABS(A2-O$5)&lt;=0.001*O$5,"Lower",ABS(A2-O$6)&lt;=0.001*O$6,"Upper",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B21">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C21">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>Ok</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="A22" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B22">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C22">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>Ok</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>Upper</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="A23" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B23">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C23">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>Ok</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="A24" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B24">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C24">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>Ok</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="A25" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B25">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C25">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D25">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>Ok</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
       </c>
       <c r="M25" t="s">
         <v>2</v>
@@ -3558,29 +3593,29 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="A26" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B26">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D26">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E26">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>Ok</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
       </c>
       <c r="L26" t="s">
         <v>13</v>
@@ -3593,29 +3628,29 @@
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="A27" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B27">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C27">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D27">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F27">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>Ok</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
       </c>
       <c r="M27">
         <v>2.8520319202830768E-3</v>
@@ -3625,237 +3660,237 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="A28" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B28">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C28">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D28">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E28">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>Ok</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="A29" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B29">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C29">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D29">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E29">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F29">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>Ok</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="A30" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B30">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C30">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D30">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E30">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F30">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>Ok</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="A31" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B31">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C31">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D31">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F31">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>Ok</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="A32" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B32">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C32">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D32">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E32">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F32">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>Ok</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="A33" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B33">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C33">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D33">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E33">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F33">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>Ok</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="A34" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B34">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C34">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D34">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E34">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F34">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>Ok</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="A35" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B35">
-        <f t="shared" ref="B35:B36" si="2">IF(OR(ABS(B17-P$5)&lt;=0.001*P$5,ABS(B17-P$6)&lt;=0.001*P$6),0,1)</f>
-        <v>1</v>
-      </c>
-      <c r="C35">
-        <f t="shared" ref="C35:C36" si="3">IF(OR(ABS(C17-Q$5)&lt;=0.001*Q$5,ABS(C17-Q$6)&lt;=0.001*Q$6),0,1)</f>
-        <v>1</v>
-      </c>
-      <c r="D35">
-        <f t="shared" ref="D35:D36" si="4">IF(OR(ABS(D17-R$5)&lt;=0.001*R$5,ABS(D17-R$6)&lt;=0.001*R$6),0,1)</f>
-        <v>1</v>
-      </c>
-      <c r="E35">
-        <f t="shared" ref="E35:E36" si="5">IF(OR(ABS(E17-S$5)&lt;=0.001*S$5,ABS(E17-S$6)&lt;=0.001*S$6),0,1)</f>
-        <v>1</v>
-      </c>
-      <c r="F35">
-        <f t="shared" ref="F35:F36" si="6">IF(OR(ABS(F17-T$5)&lt;=0.001*T$5,ABS(F17-T$6)&lt;=0.001*T$6),0,1)</f>
-        <v>1</v>
+        <v>Ok</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" ref="B35:B36" si="2">_xlfn.IFS(ABS(B17-P$5)&lt;=0.001*P$5,"Lower",ABS(B17-P$6)&lt;=0.001*P$6,"Upper",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" ref="C35:C36" si="3">_xlfn.IFS(ABS(C17-Q$5)&lt;=0.001*Q$5,"Lower",ABS(C17-Q$6)&lt;=0.001*Q$6,"Upper",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" ref="D35:D36" si="4">_xlfn.IFS(ABS(D17-R$5)&lt;=0.001*R$5,"Lower",ABS(D17-R$6)&lt;=0.001*R$6,"Upper",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" ref="E35:E36" si="5">_xlfn.IFS(ABS(E17-S$5)&lt;=0.001*S$5,"Lower",ABS(E17-S$6)&lt;=0.001*S$6,"Upper",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" ref="F35:F36" si="6">_xlfn.IFS(ABS(F17-T$5)&lt;=0.001*T$5,"Lower",ABS(F17-T$6)&lt;=0.001*T$6,"Upper",TRUE,"Ok")</f>
+        <v>Ok</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="A36" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B36">
+        <v>Ok</v>
+      </c>
+      <c r="B36" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="C36">
+        <v>Upper</v>
+      </c>
+      <c r="C36" t="str">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D36">
+        <v>Ok</v>
+      </c>
+      <c r="D36" t="str">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E36">
+        <v>Ok</v>
+      </c>
+      <c r="E36" t="str">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="F36">
+        <v>Ok</v>
+      </c>
+      <c r="F36" t="str">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>Ok</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
@@ -3870,7 +3905,7 @@
       </c>
       <c r="I37" t="e">
         <f t="shared" ref="I37" si="7">(E19-$Q$10)/($P$10-$Q$10)</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="J37">
         <v>4.9976518471215536E-2</v>
@@ -4476,12 +4511,264 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76250EAD-70B0-4177-BBAF-2C5396B4B0AE}">
+  <sheetPr codeName="Sheet7"/>
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" t="s">
+        <v>83</v>
+      </c>
+      <c r="G7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G17">
+    <sortCondition ref="A2:A17"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8BA74B9-0D47-41C5-815E-E9C7909E4600}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H32" sqref="H32:J34"/>
+      <selection activeCell="B11" sqref="B11:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5221,7 +5508,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97055BDA-DCFB-43FC-A136-A524520CA669}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:C13"/>
@@ -5351,7 +5638,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88E17877-2AD9-489D-A427-371C750705EF}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:B7"/>
@@ -5414,7 +5701,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0438E80-DC22-4133-A756-8654DAF095E1}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C13"/>
@@ -5544,7 +5831,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B238443-320F-4BFF-8BF4-24794721E863}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B7"/>

</xml_diff>

<commit_message>
Got repo back to state before running the 7 param aic check
</commit_message>
<xml_diff>
--- a/LacTissue_Final_Confirmation.xlsx
+++ b/LacTissue_Final_Confirmation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D6BFB5-C5B8-4607-8941-46EC3EA054B1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E019FE6-22A7-47F5-8E34-7593F693C46E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{DD09F72E-4848-464E-B080-00BCFE22713D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DD09F72E-4848-464E-B080-00BCFE22713D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2256,16 +2256,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2593,8 +2593,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4:T4"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4083,7 +4083,7 @@
         <v>3.3265308637097507E-2</v>
       </c>
     </row>
-    <row r="49" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F49" t="s">
         <v>0</v>
       </c>
@@ -4100,7 +4100,7 @@
         <v>1.7246081208688514E-2</v>
       </c>
     </row>
-    <row r="50" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E50" t="s">
         <v>12</v>
       </c>
@@ -4117,7 +4117,7 @@
         <v>2.6737475899886731E-2</v>
       </c>
     </row>
-    <row r="51" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F51">
         <f>STDEV(E$2,E$6,E$7,E$10)/SQRT(COUNT(E$2,E$6,E$7,E$10))</f>
         <v>1.6762636818991551E-3</v>
@@ -4131,7 +4131,15 @@
         <v>4.2168642617918499E-4</v>
       </c>
     </row>
-    <row r="52" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <f>1/C38</f>
+        <v>47.89085323251517</v>
+      </c>
+      <c r="B52">
+        <f>1/D38</f>
+        <v>49.649509441724184</v>
+      </c>
       <c r="G52" t="s">
         <v>0</v>
       </c>
@@ -4142,7 +4150,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <f>1/G50</f>
+        <v>35.954709476184604</v>
+      </c>
+      <c r="B53">
+        <f>1/H50</f>
+        <v>37.400688222938662</v>
+      </c>
       <c r="F53" t="s">
         <v>6</v>
       </c>
@@ -4159,7 +4175,7 @@
         <v>6.3762420474985501E-3</v>
       </c>
     </row>
-    <row r="54" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G54">
         <f>STDEV(F$2,F$6,F$7,F$10)/SQRT(COUNT(F$2,F$6,F$7,F$10))</f>
         <v>1.7506312950913476E-2</v>
@@ -4173,7 +4189,7 @@
         <v>6.376242047475212E-3</v>
       </c>
     </row>
-    <row r="55" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H55" t="s">
         <v>0</v>
       </c>
@@ -4184,7 +4200,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G56" t="s">
         <v>7</v>
       </c>
@@ -4201,7 +4217,7 @@
         <v>0.99702277168016751</v>
       </c>
     </row>
-    <row r="57" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H57">
         <f>STDEV(G$2,G$6,G$7,G$10)/SQRT(COUNT(G$2,G$6,G$7,G$10))</f>
         <v>3.0141188423478231E-3</v>
@@ -4215,7 +4231,7 @@
         <v>6.4424976271466709E-4</v>
       </c>
     </row>
-    <row r="58" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I58" t="s">
         <v>0</v>
       </c>
@@ -4226,7 +4242,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H59" t="s">
         <v>8</v>
       </c>
@@ -4243,7 +4259,7 @@
         <v>0.95587640865020251</v>
       </c>
     </row>
-    <row r="60" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I60">
         <f>STDEV(H$2,H$6,H$7,H$10)/SQRT(COUNT(H$2,H$6,H$7,H$10))</f>
         <v>6.7099125555603678E-3</v>
@@ -4257,7 +4273,7 @@
         <v>3.2158865150089026E-2</v>
       </c>
     </row>
-    <row r="61" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J61" t="s">
         <v>0</v>
       </c>
@@ -4268,7 +4284,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I62" t="s">
         <v>9</v>
       </c>
@@ -4285,7 +4301,7 @@
         <v>7.7706263621669117E-2</v>
       </c>
     </row>
-    <row r="63" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J63">
         <f>STDEV(I$2,I$6,I$7,I$10)/SQRT(COUNT(I$2,I$6,I$7,I$10))</f>
         <v>2.4304734850480701E-2</v>
@@ -4299,7 +4315,7 @@
         <v>9.1365500589313132E-3</v>
       </c>
     </row>
-    <row r="64" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K64" t="s">
         <v>0</v>
       </c>
@@ -4768,7 +4784,7 @@
   <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:G11"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5707,7 +5723,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C13"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>